<commit_message>
Pulling out the heavy stuff
</commit_message>
<xml_diff>
--- a/2013 ACL Training Revamp.xlsx
+++ b/2013 ACL Training Revamp.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Outline" sheetId="4" r:id="rId1"/>
     <sheet name="Punch List" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Stats" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
   <si>
     <t>Diagrams</t>
   </si>
@@ -132,26 +132,47 @@
     <t>Condense</t>
   </si>
   <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>Collect -Begin</t>
-  </si>
-  <si>
-    <t>Kickoff</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Action</t>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Audio Over</t>
+  </si>
+  <si>
+    <t>Audio Content</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>fix</t>
+  </si>
+  <si>
+    <t>Need to create output</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +203,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -260,11 +289,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -288,11 +335,96 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -781,38 +913,533 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-    </row>
+      <c r="I1" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>3</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>4</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
+        <v>5</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>6</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>7</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
+        <v>8</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
+        <v>9</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D2:H28 I17">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"fix"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="598" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>